<commit_message>
Verification Report updated and Test Record added
</commit_message>
<xml_diff>
--- a/Documents/External/ReviewRecords/Review_Sheet_Verification_Report_CommLib_Android.xlsx
+++ b/Documents/External/ReviewRecords/Review_Sheet_Verification_Report_CommLib_Android.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310250098/iCloud Drive (Archive)/Documents/Platform_Releases/Platform_Release_2.1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310250098/git/android-commlib-workspace/Source/commlib/Documents/External/ReviewRecords/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10760" yWindow="-20540" windowWidth="33600" windowHeight="20540" tabRatio="904" activeTab="1"/>
+    <workbookView xWindow="23060" yWindow="-20720" windowWidth="19660" windowHeight="19600" tabRatio="904" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Purpose</t>
   </si>
@@ -84,11 +84,59 @@
 </t>
   </si>
   <si>
-    <t>Document: CML000006 Verification Report CommLib Android, Platform Release 2.1.0
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Document: CML000006 Verification Report CommLib Android, Platform Release 2.2.0
 Product/Platform: CommLib Android/CDP2 Platform</t>
   </si>
   <si>
-    <t>Reviewer</t>
+    <t>Erik Gaal</t>
+  </si>
+  <si>
+    <t>(tab 'Logging' of this review sheet:) the column 'Reviewer' occurs twice now. Please remove one of them in the overall Review Sheet which contains the review comments of all reviewers.</t>
+  </si>
+  <si>
+    <t>For subsequent reviews, please send around pdf version of document with line numbers</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Table of Contents has not been updated</t>
+  </si>
+  <si>
+    <t>Section 1.2</t>
+  </si>
+  <si>
+    <t>Add statement to the effect that the release candidate (id?) on which the tests were performed, has been promoted to the actual release (CommLib 7.0.0), if that's in fact the case. If that is not the case, an explanation must be added what are the differences between the tested release candidate and the actual release, and how these differences have been tested, and what was the outcome of those tests.</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Section 5</t>
+  </si>
+  <si>
+    <t>Please, refer explicitly to the results of both the manual tests (in the Test Record) and of the automatic tests (in the Verification Report), and that BOTH are satisfactory.</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Superfluous column</t>
+  </si>
+  <si>
+    <t>Will be done next time</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Statement added</t>
+  </si>
+  <si>
+    <t>Text updated</t>
   </si>
 </sst>
 </file>
@@ -233,7 +281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -336,6 +384,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -352,7 +401,21 @@
     <cellStyle name="Normal 3" xfId="2"/>
     <cellStyle name="Normal 3 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -981,7 +1044,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -998,64 +1061,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="A6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G15" s="5"/>
@@ -1146,8 +1209,8 @@
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" scale="92" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;20&amp;K000000Document Review Sheet CML000006 Verification Report CommLib Android, Platform Release 2.1.0</oddHeader>
-    <oddFooter>&amp;L&amp;12Doc ID: CML000006_x000D_Version: 1.0_x000D_Status: &lt;Approved&gt;_x000D_&amp;CDocument Title:_x000D_Document Review Sheet CML000006_x000D_Template ID: CDPP-T-02000003 Template Version: 1.0_x000D_Printed copies are uncontrolled unless authenticated&amp;RAuthor: Gerard Arts_x000D_Approver: Matthijs Piek</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;20&amp;K000000Document Review Sheet CML000006 Verification Report CommLib Android, Platform Release 2.2.0</oddHeader>
+    <oddFooter>&amp;L&amp;12Doc ID: CML000006_x000D_Version: 1.0_x000D_Status: Draft_x000D_&amp;CDocument Title:_x000D_Document Review Sheet CML000006_x000D_Template ID: CDPP-T-02000003 Template Version: 1.0_x000D_Printed copies are uncontrolled unless authenticated&amp;RAuthor: Gerard Arts_x000D_Approver: Matthijs Piek</oddFooter>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1159,18 +1222,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="3"/>
-    <col min="3" max="3" width="45.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="3"/>
+    <col min="2" max="2" width="8.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="3"/>
+    <col min="4" max="4" width="45.5" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" style="3" customWidth="1"/>
@@ -1178,16 +1241,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -1195,17 +1257,17 @@
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>8</v>
@@ -1220,61 +1282,127 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+    <row r="5" spans="1:10" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="D5" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="19"/>
+      <c r="F5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>25</v>
+      </c>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" s="17"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" customFormat="1" ht="91" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="17">
+        <v>2</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="17">
+        <v>6</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="26"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="26"/>
       <c r="E10" s="18"/>
       <c r="F10" s="23"/>
@@ -1282,9 +1410,9 @@
       <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="22"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="22"/>
       <c r="E11" s="18"/>
       <c r="F11" s="23"/>
@@ -1292,9 +1420,9 @@
       <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="22"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="23"/>
@@ -1302,9 +1430,9 @@
       <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="22"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="22"/>
       <c r="E13" s="18"/>
       <c r="F13" s="23"/>
@@ -1312,9 +1440,9 @@
       <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="22"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="22"/>
       <c r="E14" s="18"/>
       <c r="F14" s="23"/>
@@ -1322,9 +1450,9 @@
       <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="27"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="27"/>
       <c r="E15" s="18"/>
       <c r="F15" s="23"/>
@@ -1332,9 +1460,9 @@
       <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="22"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="23"/>
@@ -1342,9 +1470,9 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="22"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="22"/>
       <c r="E17" s="18"/>
       <c r="F17" s="23"/>
@@ -1352,9 +1480,9 @@
       <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="17"/>
-      <c r="C18" s="22"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="22"/>
       <c r="E18" s="18"/>
       <c r="F18" s="23"/>
@@ -1362,9 +1490,9 @@
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="17"/>
-      <c r="C19" s="22"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="22"/>
       <c r="E19" s="18"/>
       <c r="F19" s="23"/>
@@ -1372,9 +1500,9 @@
       <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="17"/>
-      <c r="C20" s="22"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="22"/>
       <c r="E20" s="18"/>
       <c r="F20" s="23"/>
@@ -1382,9 +1510,9 @@
       <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="22"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="22"/>
       <c r="E21" s="18"/>
       <c r="F21" s="23"/>
@@ -1392,9 +1520,9 @@
       <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="28"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="28"/>
       <c r="E22" s="18"/>
       <c r="F22" s="23"/>
@@ -1402,9 +1530,9 @@
       <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="22"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="22"/>
       <c r="E23" s="18"/>
       <c r="F23" s="23"/>
@@ -1412,9 +1540,9 @@
       <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="22"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="22"/>
       <c r="E24" s="18"/>
       <c r="F24" s="23"/>
@@ -1422,9 +1550,9 @@
       <c r="H24" s="25"/>
     </row>
     <row r="25" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="22"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="22"/>
       <c r="E25" s="18"/>
       <c r="F25" s="23"/>
@@ -1432,9 +1560,9 @@
       <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="17"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="22"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="22"/>
       <c r="E26" s="18"/>
       <c r="F26" s="23"/>
@@ -1442,9 +1570,9 @@
       <c r="H26" s="25"/>
     </row>
     <row r="27" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="22"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="22"/>
       <c r="E27" s="18"/>
       <c r="F27" s="23"/>
@@ -1452,9 +1580,9 @@
       <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="17"/>
-      <c r="C28" s="22"/>
+      <c r="C28" s="17"/>
       <c r="D28" s="22"/>
       <c r="E28" s="18"/>
       <c r="F28" s="23"/>
@@ -1462,9 +1590,9 @@
       <c r="H28" s="25"/>
     </row>
     <row r="29" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="22"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="22"/>
       <c r="E29" s="18"/>
       <c r="F29" s="23"/>
@@ -1472,9 +1600,9 @@
       <c r="H29" s="25"/>
     </row>
     <row r="30" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="17"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="22"/>
       <c r="E30" s="18"/>
       <c r="F30" s="23"/>
@@ -1482,9 +1610,9 @@
       <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="17"/>
-      <c r="C31" s="22"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="22"/>
       <c r="E31" s="18"/>
       <c r="F31" s="23"/>
@@ -1492,9 +1620,9 @@
       <c r="H31" s="25"/>
     </row>
     <row r="32" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="28"/>
       <c r="E32" s="18"/>
       <c r="F32" s="23"/>
@@ -1502,9 +1630,9 @@
       <c r="H32" s="25"/>
     </row>
     <row r="33" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="17"/>
-      <c r="C33" s="22"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="22"/>
       <c r="E33" s="18"/>
       <c r="F33" s="23"/>
@@ -1512,9 +1640,9 @@
       <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="17"/>
-      <c r="C34" s="27"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="27"/>
       <c r="E34" s="18"/>
       <c r="F34" s="23"/>
@@ -1522,9 +1650,9 @@
       <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="22"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="22"/>
       <c r="E35" s="18"/>
       <c r="F35" s="23"/>
@@ -1532,9 +1660,9 @@
       <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="17"/>
-      <c r="C36" s="22"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="22"/>
       <c r="E36" s="18"/>
       <c r="F36" s="23"/>
@@ -1542,9 +1670,9 @@
       <c r="H36" s="25"/>
     </row>
     <row r="37" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="17"/>
-      <c r="C37" s="22"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="22"/>
       <c r="E37" s="18"/>
       <c r="F37" s="23"/>
@@ -1552,9 +1680,9 @@
       <c r="H37" s="25"/>
     </row>
     <row r="38" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="17"/>
-      <c r="C38" s="22"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="22"/>
       <c r="E38" s="18"/>
       <c r="F38" s="23"/>
@@ -1562,9 +1690,9 @@
       <c r="H38" s="25"/>
     </row>
     <row r="39" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="22"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="17"/>
       <c r="D39" s="22"/>
       <c r="E39" s="18"/>
       <c r="F39" s="23"/>
@@ -1572,9 +1700,9 @@
       <c r="H39" s="25"/>
     </row>
     <row r="40" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="29"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="22"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="22"/>
       <c r="E40" s="18"/>
       <c r="F40" s="23"/>
@@ -1582,9 +1710,9 @@
       <c r="H40" s="25"/>
     </row>
     <row r="41" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="17"/>
-      <c r="C41" s="31"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="31"/>
       <c r="E41" s="18"/>
       <c r="F41" s="23"/>
@@ -1592,9 +1720,9 @@
       <c r="H41" s="25"/>
     </row>
     <row r="42" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="17"/>
-      <c r="C42" s="22"/>
+      <c r="C42" s="17"/>
       <c r="D42" s="22"/>
       <c r="E42" s="18"/>
       <c r="F42" s="23"/>
@@ -1602,9 +1730,9 @@
       <c r="H42" s="25"/>
     </row>
     <row r="43" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="32"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="22"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="17"/>
       <c r="D43" s="22"/>
       <c r="E43" s="18"/>
       <c r="F43" s="25"/>
@@ -1612,9 +1740,9 @@
       <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="32"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="22"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="22"/>
       <c r="E44" s="18"/>
       <c r="F44" s="25"/>
@@ -1622,9 +1750,9 @@
       <c r="H44" s="25"/>
     </row>
     <row r="45" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="22"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="17"/>
       <c r="D45" s="22"/>
       <c r="E45" s="18"/>
       <c r="F45" s="25"/>
@@ -1632,9 +1760,9 @@
       <c r="H45" s="25"/>
     </row>
     <row r="46" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="32"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="22"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="17"/>
       <c r="D46" s="22"/>
       <c r="E46" s="18"/>
       <c r="F46" s="25"/>
@@ -1642,9 +1770,9 @@
       <c r="H46" s="25"/>
     </row>
     <row r="47" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="32"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="22"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="22"/>
       <c r="E47" s="18"/>
       <c r="F47" s="25"/>
@@ -1652,9 +1780,9 @@
       <c r="H47" s="25"/>
     </row>
     <row r="48" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="32"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="22"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="22"/>
       <c r="E48" s="18"/>
       <c r="F48" s="25"/>
@@ -1662,9 +1790,9 @@
       <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="32"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="22"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="22"/>
       <c r="E49" s="18"/>
       <c r="F49" s="25"/>
@@ -1672,9 +1800,9 @@
       <c r="H49" s="25"/>
     </row>
     <row r="50" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="32"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="22"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="22"/>
       <c r="E50" s="18"/>
       <c r="F50" s="25"/>
@@ -1682,9 +1810,9 @@
       <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="32"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="22"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="17"/>
       <c r="D51" s="22"/>
       <c r="E51" s="18"/>
       <c r="F51" s="25"/>
@@ -1692,9 +1820,9 @@
       <c r="H51" s="25"/>
     </row>
     <row r="52" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="32"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="22"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="17"/>
       <c r="D52" s="22"/>
       <c r="E52" s="18"/>
       <c r="F52" s="25"/>
@@ -1702,9 +1830,9 @@
       <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="32"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="22"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="17"/>
       <c r="D53" s="22"/>
       <c r="E53" s="18"/>
       <c r="F53" s="25"/>
@@ -1712,9 +1840,9 @@
       <c r="H53" s="25"/>
     </row>
     <row r="54" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="32"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="22"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="17"/>
       <c r="D54" s="22"/>
       <c r="E54" s="18"/>
       <c r="F54" s="25"/>
@@ -1722,9 +1850,9 @@
       <c r="H54" s="25"/>
     </row>
     <row r="55" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="22"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="22"/>
       <c r="E55" s="18"/>
       <c r="F55" s="25"/>
@@ -1732,9 +1860,9 @@
       <c r="H55" s="25"/>
     </row>
     <row r="56" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="32"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="22"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="17"/>
       <c r="D56" s="22"/>
       <c r="E56" s="18"/>
       <c r="F56" s="25"/>
@@ -1742,132 +1870,146 @@
       <c r="H56" s="25"/>
     </row>
     <row r="57" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="32"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="22"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="17"/>
       <c r="D57" s="22"/>
       <c r="E57" s="18"/>
       <c r="F57" s="25"/>
       <c r="G57" s="33"/>
       <c r="H57" s="25"/>
     </row>
+    <row r="58" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A58" s="34"/>
+    </row>
+    <row r="59" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A59" s="34"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
-  <conditionalFormatting sqref="E14 E5:E12">
+  <conditionalFormatting sqref="E14 E10:E12">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
+      <formula>OR(E10="S",E10="Ma",E10="mi",E10="cl",E10="Q")</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" stopIfTrue="1" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
     <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
-      <formula>OR(E5="S",E5="Ma",E5="mi",E5="cl",E5="Q")</formula>
+      <formula>OR(E15="S",E15="Ma",E15="mi",E15="cl",E15="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="28" priority="30" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="E13">
     <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
-      <formula>OR(E15="S",E15="Ma",E15="mi",E15="cl",E15="Q")</formula>
+      <formula>OR(E13="S",E13="Ma",E13="mi",E13="cl",E13="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="26" priority="28" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="E16 E18:E19 E42:E57">
     <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
-      <formula>OR(E13="S",E13="Ma",E13="mi",E13="cl",E13="Q")</formula>
+      <formula>OR(E16="S",E16="Ma",E16="mi",E16="cl",E16="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="24" priority="26" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16 E18:E19 E42:E57">
+  <conditionalFormatting sqref="E17">
     <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
-      <formula>OR(E16="S",E16="Ma",E16="mi",E16="cl",E16="Q")</formula>
+      <formula>OR(E17="S",E17="Ma",E17="mi",E17="cl",E17="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="22" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="E24">
     <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
-      <formula>OR(E17="S",E17="Ma",E17="mi",E17="cl",E17="Q")</formula>
+      <formula>OR(E24="S",E24="Ma",E24="mi",E24="cl",E24="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E41">
     <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
-      <formula>OR(E24="S",E24="Ma",E24="mi",E24="cl",E24="Q")</formula>
+      <formula>OR(E41="S",E41="Ma",E41="mi",E41="cl",E41="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
+  <conditionalFormatting sqref="E22:E23">
     <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
-      <formula>OR(E41="S",E41="Ma",E41="mi",E41="cl",E41="Q")</formula>
+      <formula>OR(E22="S",E22="Ma",E22="mi",E22="cl",E22="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E23">
+  <conditionalFormatting sqref="E20:E21">
     <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
-      <formula>OR(E22="S",E22="Ma",E22="mi",E22="cl",E22="Q")</formula>
+      <formula>OR(E20="S",E20="Ma",E20="mi",E20="cl",E20="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E21">
+  <conditionalFormatting sqref="E33 E25 E27:E31">
     <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
-      <formula>OR(E20="S",E20="Ma",E20="mi",E20="cl",E20="Q")</formula>
+      <formula>OR(E25="S",E25="Ma",E25="mi",E25="cl",E25="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33 E25 E27:E31">
+  <conditionalFormatting sqref="E34">
     <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
-      <formula>OR(E25="S",E25="Ma",E25="mi",E25="cl",E25="Q")</formula>
+      <formula>OR(E34="S",E34="Ma",E34="mi",E34="cl",E34="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
+  <conditionalFormatting sqref="E32">
     <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
-      <formula>OR(E34="S",E34="Ma",E34="mi",E34="cl",E34="Q")</formula>
+      <formula>OR(E32="S",E32="Ma",E32="mi",E32="cl",E32="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E35 E37:E40">
     <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
-      <formula>OR(E32="S",E32="Ma",E32="mi",E32="cl",E32="Q")</formula>
+      <formula>OR(E35="S",E35="Ma",E35="mi",E35="cl",E35="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35 E37:E40">
+  <conditionalFormatting sqref="E36">
     <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>OR(E35="S",E35="Ma",E35="mi",E35="cl",E35="Q")</formula>
+      <formula>OR(E36="S",E36="Ma",E36="mi",E36="cl",E36="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="E26">
     <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>OR(E36="S",E36="Ma",E36="mi",E36="cl",E36="Q")</formula>
+      <formula>OR(E26="S",E26="Ma",E26="mi",E26="cl",E26="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
+  <conditionalFormatting sqref="E5:E9">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>OR(E26="S",E26="Ma",E26="mi",E26="cl",E26="Q")</formula>
+      <formula>OR(E5="S",E5="Ma",E5="mi",E5="cl",E5="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
@@ -1896,12 +2038,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006DF22D4ED0D65744A5324CFBF61E7267" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c7d39199afebea215da257a1a8442a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2015,16 +2166,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2039,7 +2189,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFFD0C5-71AF-43FC-BB9C-C9954D60B2E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2053,12 +2203,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>